<commit_message>
P6- Falta Arreglar Neg. Binarios
</commit_message>
<xml_diff>
--- a/Tabop.xlsx
+++ b/Tabop.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Franco\Escritorio\JOSUE\Universidad\5° Semestre\Seminario de Traductores de Leguaje 1\Practica1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\OneDrive\Documents\Practica1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E9987C-6507-4386-95CA-1EBA344F52EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C1AB468-9176-4315-BAA3-06BEDBCB5463}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="240" windowWidth="14220" windowHeight="15360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1429" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1430" uniqueCount="301">
   <si>
     <t>Conjunto de Instrucciones de HC12</t>
   </si>
@@ -927,7 +927,7 @@
     <t>B7C6</t>
   </si>
   <si>
-    <t>IDAA</t>
+    <t>Cero</t>
   </si>
 </sst>
 </file>
@@ -1303,8 +1303,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F379"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="A171" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A204" sqref="A204"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2570,8 +2570,8 @@
       <c r="C66" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D66" s="3">
-        <v>0</v>
+      <c r="D66" s="3" t="s">
+        <v>300</v>
       </c>
       <c r="E66" s="3">
         <v>0</v>
@@ -5242,7 +5242,7 @@
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200" s="3" t="s">
-        <v>300</v>
+        <v>156</v>
       </c>
       <c r="B200" s="3" t="s">
         <v>2</v>
@@ -5262,7 +5262,7 @@
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" s="3" t="s">
-        <v>300</v>
+        <v>156</v>
       </c>
       <c r="B201" s="3" t="s">
         <v>2</v>
@@ -5282,7 +5282,7 @@
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" s="3" t="s">
-        <v>300</v>
+        <v>156</v>
       </c>
       <c r="B202" s="3" t="s">
         <v>2</v>
@@ -5302,7 +5302,7 @@
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" s="3" t="s">
-        <v>300</v>
+        <v>156</v>
       </c>
       <c r="B203" s="3" t="s">
         <v>2</v>
@@ -5322,7 +5322,7 @@
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" s="3" t="s">
-        <v>300</v>
+        <v>156</v>
       </c>
       <c r="B204" s="3" t="s">
         <v>2</v>

</xml_diff>